<commit_message>
Search + Delete User+Image
</commit_message>
<xml_diff>
--- a/Kịch-bản-KTPM (1).xlsx
+++ b/Kịch-bản-KTPM (1).xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="100">
   <si>
     <t>Function</t>
   </si>
@@ -102,7 +102,7 @@
     <t>Fail</t>
   </si>
   <si>
-    <t>I can login with UpperCase Username</t>
+    <t>Bug "login with UpperCase Username"</t>
   </si>
   <si>
     <t>loginWithUppercasePassword</t>
@@ -132,7 +132,7 @@
 Password:admin123 </t>
   </si>
   <si>
-    <t>I can login with lowerCase Username</t>
+    <t>Bug "login with lowerCase Username"</t>
   </si>
   <si>
     <t>loginWithSpaceCharacter</t>
@@ -294,30 +294,68 @@
     <t>findWithUsername</t>
   </si>
   <si>
+    <t xml:space="preserve">Tìm kiếm user theo username </t>
+  </si>
+  <si>
     <t xml:space="preserve">
+username : Admin</t>
+  </si>
+  <si>
+    <t>user có username="Admin" hiện ra</t>
+  </si>
+  <si>
+    <t>findWithUserRole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tìm kiếm user theo vai trò userRole </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+role:Admin</t>
+  </si>
+  <si>
+    <t>user có role="Admin" hiện ra</t>
+  </si>
+  <si>
+    <t>findWithEmployee_Name</t>
+  </si>
+  <si>
+    <t>Tìm kiếm user theo Employee Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Employee Name : Alice Duval
 </t>
   </si>
   <si>
-    <t>findWithUserRole</t>
-  </si>
-  <si>
-    <t>findWithEmployee_Name</t>
+    <t>user thuộc về Employee ="Alice Duval" hiện ra</t>
+  </si>
+  <si>
+    <t>findWithStatus</t>
+  </si>
+  <si>
+    <t>Tìm kiếm user theo trạng thái hoạt động</t>
+  </si>
+  <si>
+    <t>Status : Disable</t>
+  </si>
+  <si>
+    <t>user đang ở trạng thái disable hiện ra</t>
+  </si>
+  <si>
+    <t>deteleUser</t>
+  </si>
+  <si>
+    <t>Kiểm tra chức năng xóa user có hoạt động?</t>
+  </si>
+  <si>
+    <t>Exist User</t>
+  </si>
+  <si>
+    <t>user bị xóa khỏi table</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Vào chức năng quản trị viên -&gt;  user managament -&gt; System User -&gt;  add(thêm mới)-&gt; nhập thông tin user-&gt; save
-Kiểm tra chức năng xóa 
-+chọn một user bằng cách tích vào ô trống bên trái cùng -&gt; chọn delete
-+Kiểm tra xem tài khoản vừa xóa đã mất chưa
-Kiểm tra chức năng tìm kiếm( share)
-+ nhập từ trường username
-+nhập từ trường user Role( vai trò ng dùng)
-+Nhập từ trường Employee Name( tên nhân viên)</t>
-  </si>
-  <si>
-    <t>Tài khoản cần xóa bị xóa khỏi table</t>
   </si>
   <si>
     <t>QUẢN LÍ NHÂN
@@ -344,6 +382,9 @@
     <t>Kiểm tra chức năng xóa 
 +chọn một user bằng cách tích vào ô trống bên trái cùng -&gt; chọn delete
 +Kiểm tra xem tài khoản vừa xóa đã mất chưa</t>
+  </si>
+  <si>
+    <t>Tài khoản cần xóa bị xóa khỏi table</t>
   </si>
 </sst>
 </file>
@@ -352,8 +393,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="23">
@@ -385,14 +426,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -402,14 +435,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -417,6 +443,29 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -430,17 +479,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -461,6 +525,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -469,16 +540,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -486,7 +557,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -498,36 +569,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -538,13 +579,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -556,55 +669,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -616,109 +747,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -868,47 +909,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -937,6 +944,51 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -954,29 +1006,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -986,136 +1027,135 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1131,7 +1171,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1160,9 +1199,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -1170,7 +1206,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1180,6 +1215,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1194,12 +1232,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1523,10 +1555,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:AH44"/>
+  <dimension ref="A2:AH47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1535,74 +1567,72 @@
     <col min="2" max="2" width="6.22222222222222" customWidth="1"/>
     <col min="3" max="3" width="10.287037037037" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="11.2222222222222" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="31.6666666666667" style="2" customWidth="1"/>
-    <col min="6" max="6" width="87.1111111111111" style="3" customWidth="1"/>
+    <col min="5" max="5" width="31.6666666666667" style="1" customWidth="1"/>
+    <col min="6" max="6" width="87.1111111111111" style="2" customWidth="1"/>
     <col min="7" max="7" width="25" customWidth="1"/>
     <col min="8" max="8" width="48.8888888888889" customWidth="1"/>
     <col min="9" max="9" width="13.287037037037" customWidth="1"/>
     <col min="10" max="10" width="13.712962962963" customWidth="1"/>
-    <col min="11" max="11" width="13.287037037037" style="4" customWidth="1"/>
+    <col min="11" max="11" width="13.287037037037" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" ht="31.2" spans="1:11">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="8" t="s">
+      <c r="D2" s="6"/>
+      <c r="E2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="11"/>
-      <c r="K2" s="36" t="s">
+      <c r="J2" s="9"/>
+      <c r="K2" s="33" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="31.2" spans="1:34">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="10">
         <v>1</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="8" t="s">
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="12"/>
-      <c r="K3" s="17" t="s">
-        <v>14</v>
-      </c>
+      <c r="J3" s="10"/>
+      <c r="K3" s="15"/>
       <c r="L3"/>
       <c r="M3"/>
       <c r="N3"/>
@@ -1628,31 +1658,29 @@
       <c r="AH3"/>
     </row>
     <row r="4" s="1" customFormat="1" ht="43.2" spans="1:34">
-      <c r="A4" s="18"/>
-      <c r="B4" s="12">
+      <c r="A4" s="16"/>
+      <c r="B4" s="10">
         <v>2</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="8" t="s">
+      <c r="C4" s="11"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="12"/>
-      <c r="K4" s="17" t="s">
-        <v>14</v>
-      </c>
+      <c r="J4" s="10"/>
+      <c r="K4" s="15"/>
       <c r="L4"/>
       <c r="M4"/>
       <c r="N4"/>
@@ -1678,19 +1706,19 @@
       <c r="AH4"/>
     </row>
     <row r="5" s="1" customFormat="1" ht="43.2" spans="1:34">
-      <c r="A5" s="18"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="1">
         <v>3</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="8" t="s">
+      <c r="C5" s="11"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="18" t="s">
         <v>21</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -1699,8 +1727,7 @@
       <c r="I5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="1"/>
-      <c r="K5" s="37"/>
+      <c r="K5" s="26"/>
       <c r="L5"/>
       <c r="M5"/>
       <c r="N5"/>
@@ -1726,29 +1753,28 @@
       <c r="AH5"/>
     </row>
     <row r="6" s="1" customFormat="1" ht="43.2" spans="1:34">
-      <c r="A6" s="18"/>
-      <c r="B6" s="21">
+      <c r="A6" s="16"/>
+      <c r="B6" s="19">
         <v>4</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="8" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="18" t="s">
         <v>25</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K6" s="37" t="s">
+      <c r="K6" s="26" t="s">
         <v>27</v>
       </c>
       <c r="L6"/>
@@ -1776,19 +1802,19 @@
       <c r="AH6"/>
     </row>
     <row r="7" s="1" customFormat="1" ht="43.2" spans="1:34">
-      <c r="A7" s="18"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="1">
         <v>5</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="8" t="s">
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="18" t="s">
         <v>30</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -1797,7 +1823,7 @@
       <c r="I7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="37"/>
+      <c r="K7" s="26"/>
       <c r="L7"/>
       <c r="M7"/>
       <c r="N7"/>
@@ -1823,19 +1849,19 @@
       <c r="AH7"/>
     </row>
     <row r="8" s="1" customFormat="1" ht="31.2" spans="1:34">
-      <c r="A8" s="18"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="1">
         <v>6</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="8" t="s">
+      <c r="C8" s="11"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="18" t="s">
         <v>30</v>
       </c>
       <c r="H8" s="1" t="s">
@@ -1844,7 +1870,7 @@
       <c r="I8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="37"/>
+      <c r="K8" s="26"/>
       <c r="L8"/>
       <c r="M8"/>
       <c r="N8"/>
@@ -1870,19 +1896,19 @@
       <c r="AH8"/>
     </row>
     <row r="9" s="1" customFormat="1" ht="43.2" spans="1:34">
-      <c r="A9" s="18"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="1">
         <v>7</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="8" t="s">
+      <c r="C9" s="11"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="G9" s="18" t="s">
         <v>35</v>
       </c>
       <c r="H9" s="1" t="s">
@@ -1891,7 +1917,7 @@
       <c r="I9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K9" s="37" t="s">
+      <c r="K9" s="26" t="s">
         <v>36</v>
       </c>
       <c r="L9"/>
@@ -1919,19 +1945,19 @@
       <c r="AH9"/>
     </row>
     <row r="10" s="1" customFormat="1" ht="31.2" spans="1:34">
-      <c r="A10" s="18"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="1">
         <v>8</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="8" t="s">
+      <c r="C10" s="11"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="20" t="s">
+      <c r="G10" s="18" t="s">
         <v>39</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -1940,7 +1966,7 @@
       <c r="I10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K10" s="37"/>
+      <c r="K10" s="26"/>
       <c r="L10"/>
       <c r="M10"/>
       <c r="N10"/>
@@ -1966,18 +1992,18 @@
       <c r="AH10"/>
     </row>
     <row r="11" s="1" customFormat="1" ht="15.6" spans="1:34">
-      <c r="A11" s="18"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="1">
         <v>9</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="8" t="s">
+      <c r="C11" s="11"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="23"/>
-      <c r="K11" s="37"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="20"/>
+      <c r="K11" s="26"/>
       <c r="L11"/>
       <c r="M11"/>
       <c r="N11"/>
@@ -2003,16 +2029,16 @@
       <c r="AH11"/>
     </row>
     <row r="12" s="1" customFormat="1" ht="15.6" spans="1:34">
-      <c r="A12" s="18"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="1">
         <v>10</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="23"/>
-      <c r="K12" s="37"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="20"/>
+      <c r="K12" s="26"/>
       <c r="L12"/>
       <c r="M12"/>
       <c r="N12"/>
@@ -2038,16 +2064,16 @@
       <c r="AH12"/>
     </row>
     <row r="13" s="1" customFormat="1" ht="15.6" spans="1:34">
-      <c r="A13" s="18"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="1">
         <v>11</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="23"/>
-      <c r="K13" s="37"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="20"/>
+      <c r="K13" s="26"/>
       <c r="L13"/>
       <c r="M13"/>
       <c r="N13"/>
@@ -2073,559 +2099,621 @@
       <c r="AH13"/>
     </row>
     <row r="14" customFormat="1" ht="15.6" spans="1:11">
-      <c r="A14" s="24"/>
-      <c r="B14" s="25">
+      <c r="A14" s="21"/>
+      <c r="B14" s="22">
         <v>12</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="38"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="34"/>
     </row>
     <row r="15" ht="100.8" spans="1:11">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="28">
+      <c r="B15" s="23">
         <v>13</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="8" t="s">
+      <c r="C15" s="11"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="F15" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="29" t="s">
+      <c r="G15" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="H15" s="28" t="s">
+      <c r="H15" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="I15" s="28" t="s">
+      <c r="I15" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="J15" s="28"/>
-      <c r="K15" s="39"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="34"/>
     </row>
     <row r="16" ht="100.8" spans="1:11">
-      <c r="A16" s="27"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="1">
         <v>14</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="8" t="s">
+      <c r="C16" s="11"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="G16" s="29" t="s">
+      <c r="G16" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="H16" s="30" t="s">
+      <c r="H16" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="I16" s="28" t="s">
+      <c r="I16" s="23" t="s">
         <v>14</v>
       </c>
       <c r="J16" s="1"/>
-      <c r="K16" s="37"/>
+      <c r="K16" s="26"/>
     </row>
     <row r="17" ht="100.8" spans="1:11">
-      <c r="A17" s="31"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="1">
         <v>15</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="8" t="s">
+      <c r="C17" s="11"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="F17" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="G17" s="29" t="s">
+      <c r="G17" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="H17" s="30" t="s">
+      <c r="H17" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="I17" s="28" t="s">
+      <c r="I17" s="23" t="s">
         <v>14</v>
       </c>
       <c r="J17" s="1"/>
-      <c r="K17" s="37"/>
+      <c r="K17" s="26"/>
     </row>
     <row r="18" ht="100.8" spans="1:11">
-      <c r="A18" s="31"/>
+      <c r="A18" s="24"/>
       <c r="B18" s="1">
         <v>16</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="8" t="s">
+      <c r="C18" s="11"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="G18" s="29" t="s">
+      <c r="G18" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="H18" s="30" t="s">
+      <c r="H18" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="I18" s="28" t="s">
+      <c r="I18" s="23" t="s">
         <v>14</v>
       </c>
       <c r="J18" s="1"/>
-      <c r="K18" s="37"/>
+      <c r="K18" s="26"/>
     </row>
     <row r="19" ht="100.8" spans="1:11">
-      <c r="A19" s="31"/>
+      <c r="A19" s="24"/>
       <c r="B19" s="1">
         <v>17</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="8" t="s">
+      <c r="C19" s="11"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F19" s="15" t="s">
+      <c r="F19" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="G19" s="29" t="s">
+      <c r="G19" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="I19" s="28" t="s">
+      <c r="I19" s="23" t="s">
         <v>14</v>
       </c>
       <c r="J19" s="1"/>
-      <c r="K19" s="37"/>
+      <c r="K19" s="26"/>
     </row>
     <row r="20" ht="100.8" spans="1:11">
-      <c r="A20" s="31"/>
+      <c r="A20" s="24"/>
       <c r="B20" s="1">
         <v>18</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="8" t="s">
+      <c r="C20" s="11"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="F20" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="G20" s="29" t="s">
+      <c r="G20" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="I20" s="28" t="s">
+      <c r="I20" s="23" t="s">
         <v>14</v>
       </c>
       <c r="J20" s="1"/>
-      <c r="K20" s="37"/>
+      <c r="K20" s="26"/>
     </row>
     <row r="21" ht="100.8" spans="1:11">
-      <c r="A21" s="31"/>
+      <c r="A21" s="24"/>
       <c r="B21" s="1">
         <v>19</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="8" t="s">
+      <c r="C21" s="11"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F21" s="15" t="s">
+      <c r="F21" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="G21" s="29" t="s">
+      <c r="G21" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="H21" s="30" t="s">
+      <c r="H21" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="I21" s="28" t="s">
+      <c r="I21" s="23" t="s">
         <v>14</v>
       </c>
       <c r="J21" s="1"/>
-      <c r="K21" s="37"/>
+      <c r="K21" s="26"/>
     </row>
     <row r="22" ht="100.8" spans="1:11">
-      <c r="A22" s="31"/>
+      <c r="A22" s="24"/>
       <c r="B22" s="1">
         <v>20</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="8" t="s">
+      <c r="C22" s="11"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F22" s="15" t="s">
+      <c r="F22" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="G22" s="29" t="s">
+      <c r="G22" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="H22" s="30" t="s">
+      <c r="H22" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="I22" s="28" t="s">
+      <c r="I22" s="23" t="s">
         <v>14</v>
       </c>
       <c r="J22" s="1"/>
-      <c r="K22" s="37"/>
+      <c r="K22" s="26"/>
     </row>
     <row r="23" ht="28.8" spans="1:11">
-      <c r="A23" s="31"/>
+      <c r="A23" s="24"/>
       <c r="B23" s="1">
         <v>21</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="8" t="s">
+      <c r="C23" s="11"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F23" s="15"/>
-      <c r="G23" s="29" t="s">
+      <c r="F23" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="H23" s="30"/>
-      <c r="I23" s="1"/>
+      <c r="G23" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="H23" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="J23" s="1"/>
-      <c r="K23" s="37"/>
+      <c r="K23" s="26"/>
     </row>
     <row r="24" ht="28.8" spans="1:11">
-      <c r="A24" s="31"/>
+      <c r="A24" s="24"/>
       <c r="B24" s="1">
         <v>22</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="F24" s="15"/>
-      <c r="G24" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="H24" s="30"/>
-      <c r="I24" s="1"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="H24" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="J24" s="1"/>
-      <c r="K24" s="37"/>
-    </row>
-    <row r="25" ht="28.8" spans="1:11">
-      <c r="A25" s="31"/>
+      <c r="K24" s="26"/>
+    </row>
+    <row r="25" ht="43.2" spans="1:11">
+      <c r="A25" s="24"/>
       <c r="B25" s="1">
         <v>23</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="F25" s="15"/>
-      <c r="G25" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="H25" s="30"/>
-      <c r="I25" s="1"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="G25" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="H25" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="J25" s="1"/>
-      <c r="K25" s="37"/>
-    </row>
-    <row r="26" ht="114" customHeight="1" spans="1:11">
-      <c r="A26" s="32"/>
-      <c r="B26" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="G26" s="23"/>
-      <c r="H26" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I26" s="1"/>
+      <c r="K25" s="26"/>
+    </row>
+    <row r="26" ht="15.6" spans="1:11">
+      <c r="A26" s="27"/>
+      <c r="B26" s="1">
+        <v>24</v>
+      </c>
+      <c r="C26" s="11"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="G26" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="H26" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="J26" s="1"/>
-      <c r="K26" s="37"/>
-    </row>
-    <row r="27" ht="43.2" spans="1:11">
-      <c r="A27" s="33" t="s">
-        <v>79</v>
-      </c>
+      <c r="K26" s="26"/>
+    </row>
+    <row r="27" ht="15.6" spans="1:11">
+      <c r="A27" s="27"/>
       <c r="B27" s="1">
-        <v>15</v>
-      </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="G27" s="23"/>
-      <c r="H27" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="I27" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="C27" s="11"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="G27" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="H27" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="J27" s="1"/>
-      <c r="K27" s="37"/>
-    </row>
-    <row r="28" ht="28.8" spans="1:11">
+      <c r="K27" s="26"/>
+    </row>
+    <row r="28" ht="15.6" spans="1:11">
       <c r="A28" s="27"/>
-      <c r="B28" s="1">
-        <v>16</v>
-      </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="G28" s="23"/>
-      <c r="H28" s="30" t="s">
-        <v>83</v>
-      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="26"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
-      <c r="K28" s="37"/>
-    </row>
-    <row r="29" ht="43.2" spans="1:11">
-      <c r="A29" s="32"/>
-      <c r="B29" s="1">
-        <v>17</v>
-      </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="G29" s="23"/>
-      <c r="H29" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="K28" s="26"/>
+    </row>
+    <row r="29" ht="114" customHeight="1" spans="1:11">
+      <c r="A29" s="29"/>
+      <c r="B29" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" s="11"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
-      <c r="K29" s="37"/>
-    </row>
-    <row r="30" ht="15.6" spans="1:11">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="1"/>
+      <c r="K29" s="26"/>
+    </row>
+    <row r="30" ht="43.2" spans="1:11">
+      <c r="A30" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="1">
+        <v>15</v>
+      </c>
+      <c r="C30" s="11"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="G30" s="20"/>
+      <c r="H30" s="26" t="s">
+        <v>95</v>
+      </c>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
-      <c r="K30" s="37"/>
-    </row>
-    <row r="31" ht="15.6" spans="1:11">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="1"/>
+      <c r="K30" s="26"/>
+    </row>
+    <row r="31" ht="28.8" spans="1:11">
+      <c r="A31" s="24"/>
+      <c r="B31" s="1">
+        <v>16</v>
+      </c>
+      <c r="C31" s="11"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="G31" s="20"/>
+      <c r="H31" s="26" t="s">
+        <v>97</v>
+      </c>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
-      <c r="K31" s="37"/>
-    </row>
-    <row r="32" ht="15.6" spans="1:11">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="1"/>
+      <c r="K31" s="26"/>
+    </row>
+    <row r="32" ht="43.2" spans="1:11">
+      <c r="A32" s="29"/>
+      <c r="B32" s="1">
+        <v>17</v>
+      </c>
+      <c r="C32" s="11"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="G32" s="20"/>
+      <c r="H32" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
-      <c r="K32" s="37"/>
+      <c r="K32" s="26"/>
     </row>
     <row r="33" ht="15.6" spans="1:11">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="23"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="7"/>
+      <c r="G33" s="20"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
-      <c r="K33" s="37"/>
+      <c r="K33" s="26"/>
     </row>
     <row r="34" ht="15.6" spans="1:11">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="23"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="7"/>
+      <c r="G34" s="20"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
-      <c r="K34" s="37"/>
+      <c r="K34" s="26"/>
     </row>
     <row r="35" ht="15.6" spans="1:11">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="23"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="7"/>
+      <c r="G35" s="20"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
-      <c r="K35" s="37"/>
+      <c r="K35" s="26"/>
     </row>
     <row r="36" ht="15.6" spans="1:11">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="23"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="7"/>
+      <c r="G36" s="20"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
-      <c r="K36" s="37"/>
+      <c r="K36" s="26"/>
     </row>
     <row r="37" ht="15.6" spans="1:11">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="23"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="7"/>
+      <c r="G37" s="20"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
-      <c r="K37" s="37"/>
+      <c r="K37" s="26"/>
     </row>
     <row r="38" ht="15.6" spans="1:11">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="23"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="7"/>
+      <c r="G38" s="20"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
-      <c r="K38" s="37"/>
+      <c r="K38" s="26"/>
     </row>
     <row r="39" ht="15.6" spans="1:11">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="23"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="7"/>
+      <c r="G39" s="20"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
-      <c r="K39" s="37"/>
+      <c r="K39" s="26"/>
     </row>
     <row r="40" ht="15.6" spans="1:11">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="23"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="7"/>
+      <c r="G40" s="20"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
-      <c r="K40" s="37"/>
+      <c r="K40" s="26"/>
     </row>
     <row r="41" ht="15.6" spans="1:11">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="23"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="7"/>
+      <c r="G41" s="20"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
-      <c r="K41" s="37"/>
+      <c r="K41" s="26"/>
     </row>
     <row r="42" ht="15.6" spans="1:11">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="23"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="7"/>
+      <c r="G42" s="20"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
-      <c r="K42" s="37"/>
+      <c r="K42" s="26"/>
     </row>
     <row r="43" ht="15.6" spans="1:11">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="23"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="7"/>
+      <c r="G43" s="20"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
-      <c r="K43" s="37"/>
+      <c r="K43" s="26"/>
     </row>
     <row r="44" ht="15.6" spans="1:11">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="35"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="23"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="7"/>
+      <c r="G44" s="20"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
-      <c r="K44" s="37"/>
+      <c r="K44" s="26"/>
+    </row>
+    <row r="45" ht="15.6" spans="1:11">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="7"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="26"/>
+    </row>
+    <row r="46" ht="15.6" spans="1:11">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="7"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="26"/>
+    </row>
+    <row r="47" ht="15.6" spans="1:11">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="7"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="A3:A13"/>
-    <mergeCell ref="A15:A26"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="C2:D44"/>
+    <mergeCell ref="A15:A29"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="C2:D47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>

</xml_diff>

<commit_message>
Edit test cases for employee management functions
</commit_message>
<xml_diff>
--- a/Kịch-bản-KTPM (1).xlsx
+++ b/Kịch-bản-KTPM (1).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335"/>
+    <workbookView windowWidth="19200" windowHeight="7070"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="125">
   <si>
     <t>Function</t>
   </si>
@@ -34,10 +34,10 @@
     <t>Test Data</t>
   </si>
   <si>
-    <t>Expected results(kq mong muốn)</t>
-  </si>
-  <si>
-    <t>Testing result(pass/faile)</t>
+    <t>Expected results(kết quả mong muốn)</t>
+  </si>
+  <si>
+    <t>Testing result(pass/fail)</t>
   </si>
   <si>
     <t>ReasonFail(Fail)</t>
@@ -376,29 +376,98 @@
  VIÊN</t>
   </si>
   <si>
-    <t>Kiểm tra chức năng thêm nhân viên 
-+nhập tất cả thông tin yêu cầu --&gt; add 
-Kiểm tra xem thông tin được lưu.</t>
-  </si>
-  <si>
-    <t>lưu được thông tin nhân vien mới 
-vào bảng danh sách nhân viên</t>
-  </si>
-  <si>
-    <t>Kiểm tra chức năng tìm kiếm 
-+Nhập vào trường  tương ứng thông tin cần tìm .-&gt; share</t>
-  </si>
-  <si>
-    <t>kết quả cần tìm liên quan gần đúng
-hoặc đúng được lọc ra</t>
-  </si>
-  <si>
-    <t>Kiểm tra chức năng xóa 
-+chọn một user bằng cách tích vào ô trống bên trái cùng -&gt; chọn delete
-+Kiểm tra xem tài khoản vừa xóa đã mất chưa</t>
-  </si>
-  <si>
-    <t>Tài khoản cần xóa bị xóa khỏi table</t>
+    <t>testAddEmployee</t>
+  </si>
+  <si>
+    <t>Thêm nhân viên mới cùng với tài khoản nhân viên mới đó có giá trị hợp lệ</t>
+  </si>
+  <si>
+    <t>firstName: John
+lastName: Karth
+employeeId: 0222
+user_name: johnkarth0222
+user_password: jkpwdacb.1@3
+re_password:  jkpwdacb.1@3
+status: Enabled</t>
+  </si>
+  <si>
+    <t>Thông tin nhân viên mới được thêm vào
+Hiện ra trang thông tin chi tiết của nhân viên mới được thêm vào</t>
+  </si>
+  <si>
+    <t>testAddEmployeeIDExist</t>
+  </si>
+  <si>
+    <t>Thêm nhân viên với mã nhân viên đã tồn tại</t>
+  </si>
+  <si>
+    <t>firstName: John
+lastName: Karth
+employeeId: 0222</t>
+  </si>
+  <si>
+    <t>Hiện thông báo "Failed To Save: Employee Id Exists"</t>
+  </si>
+  <si>
+    <t>testSearchEmployeeNameExist</t>
+  </si>
+  <si>
+    <t>Tìm kiếm nhân viên với tên đã tồn tại</t>
+  </si>
+  <si>
+    <t>empsearch_employee_name_empName: John</t>
+  </si>
+  <si>
+    <t>Hiện thông tin của các tài khoản có tên là John</t>
+  </si>
+  <si>
+    <t>testSearchEmployeeNameAndIDExist</t>
+  </si>
+  <si>
+    <t>Tìm kiếm nhân viên với tên và ID đã tồn tại</t>
+  </si>
+  <si>
+    <t>empsearch_id: 0011
+empsearch_employee_name_empName: John</t>
+  </si>
+  <si>
+    <t>Hiện thông tin của các tài khoản có tên là John
+và có mã nhân viên là 0011</t>
+  </si>
+  <si>
+    <t>testSearchEmployeeNameNotExist</t>
+  </si>
+  <si>
+    <t>Tìm kiếm nhân viên với tên chưa tồn tại</t>
+  </si>
+  <si>
+    <t>empsearch_employee_name_empName: Johnathan</t>
+  </si>
+  <si>
+    <t>Hiện thông báo "No Records Found" ở table</t>
+  </si>
+  <si>
+    <t>testSearchEmployeeNameAndIDNotExist</t>
+  </si>
+  <si>
+    <t>Tìm kiếm nhân viên với tên và ID chưa tồn tại</t>
+  </si>
+  <si>
+    <t>empsearch_id: 1001
+empsearch_employee_name_empName: Stella</t>
+  </si>
+  <si>
+    <t>testDeleteEmployee</t>
+  </si>
+  <si>
+    <t>Xóa nhân viên với mã nhân viên đã tồn tại</t>
+  </si>
+  <si>
+    <t>empsearch_id: 0118</t>
+  </si>
+  <si>
+    <t>HIện thông báo "Successfully Deleted"
+Hiện thông báo "No Records Found" ở table</t>
   </si>
 </sst>
 </file>
@@ -406,14 +475,22 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -440,20 +517,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -463,7 +526,7 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -471,14 +534,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -501,6 +557,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -512,6 +576,13 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -532,10 +603,17 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -549,14 +627,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -578,13 +648,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -593,13 +670,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -611,31 +814,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -645,140 +872,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -923,26 +1018,24 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -964,9 +1057,35 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1003,17 +1122,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -1023,7 +1131,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1041,211 +1149,296 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1568,82 +1761,82 @@
   <sheetPr/>
   <dimension ref="A2:AH47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.4259259259259" customWidth="1"/>
-    <col min="2" max="2" width="6.22222222222222" customWidth="1"/>
-    <col min="3" max="3" width="10.287037037037" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="11.2222222222222" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="31.6666666666667" style="1" customWidth="1"/>
-    <col min="6" max="6" width="87.1111111111111" style="2" customWidth="1"/>
-    <col min="7" max="7" width="25" customWidth="1"/>
-    <col min="8" max="8" width="48.8888888888889" customWidth="1"/>
-    <col min="9" max="9" width="13.287037037037" customWidth="1"/>
-    <col min="10" max="10" width="13.712962962963" customWidth="1"/>
-    <col min="11" max="11" width="13.287037037037" style="3" customWidth="1"/>
+    <col min="1" max="1" width="15.4272727272727" customWidth="1"/>
+    <col min="2" max="2" width="6.21818181818182" customWidth="1"/>
+    <col min="3" max="3" width="10.2909090909091" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="11.2181818181818" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="39.2818181818182" style="2" customWidth="1"/>
+    <col min="6" max="6" width="87.1090909090909" style="3" customWidth="1"/>
+    <col min="7" max="7" width="42.1272727272727" customWidth="1"/>
+    <col min="8" max="8" width="48.8909090909091" style="4" customWidth="1"/>
+    <col min="9" max="9" width="13.2909090909091" style="4" customWidth="1"/>
+    <col min="10" max="10" width="13.7090909090909" style="4" customWidth="1"/>
+    <col min="11" max="11" width="21.9090909090909" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" ht="31.2" spans="1:11">
-      <c r="A2" s="4" t="s">
+    <row r="2" s="1" customFormat="1" ht="37" spans="1:11">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="32" t="s">
+      <c r="J2" s="51"/>
+      <c r="K2" s="52" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" ht="31.2" spans="1:34">
-      <c r="A3" s="9" t="s">
+    <row r="3" s="2" customFormat="1" ht="29" spans="1:34">
+      <c r="A3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="13">
         <v>1</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="7" t="s">
+      <c r="C3" s="14"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="15"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="19"/>
       <c r="L3"/>
       <c r="M3"/>
       <c r="N3"/>
@@ -1668,30 +1861,30 @@
       <c r="AG3"/>
       <c r="AH3"/>
     </row>
-    <row r="4" s="1" customFormat="1" ht="43.2" spans="1:34">
-      <c r="A4" s="16"/>
-      <c r="B4" s="10">
+    <row r="4" s="2" customFormat="1" ht="43.5" spans="1:34">
+      <c r="A4" s="20"/>
+      <c r="B4" s="13">
         <v>2</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="7" t="s">
+      <c r="C4" s="14"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="10"/>
-      <c r="K4" s="15"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="19"/>
       <c r="L4"/>
       <c r="M4"/>
       <c r="N4"/>
@@ -1716,29 +1909,30 @@
       <c r="AG4"/>
       <c r="AH4"/>
     </row>
-    <row r="5" s="1" customFormat="1" ht="31.2" spans="1:34">
-      <c r="A5" s="16"/>
-      <c r="B5" s="1">
+    <row r="5" s="2" customFormat="1" ht="31" spans="1:34">
+      <c r="A5" s="20"/>
+      <c r="B5" s="2">
         <v>3</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="7" t="s">
+      <c r="C5" s="14"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="27"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="34"/>
       <c r="L5"/>
       <c r="M5"/>
       <c r="N5"/>
@@ -1763,30 +1957,30 @@
       <c r="AG5"/>
       <c r="AH5"/>
     </row>
-    <row r="6" s="1" customFormat="1" ht="31.2" spans="1:34">
-      <c r="A6" s="16"/>
-      <c r="B6" s="19">
+    <row r="6" s="2" customFormat="1" ht="31" spans="1:34">
+      <c r="A6" s="20"/>
+      <c r="B6" s="25">
         <v>4</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="7" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="27"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="34"/>
       <c r="L6"/>
       <c r="M6"/>
       <c r="N6"/>
@@ -1811,29 +2005,30 @@
       <c r="AG6"/>
       <c r="AH6"/>
     </row>
-    <row r="7" s="1" customFormat="1" ht="31.2" spans="1:34">
-      <c r="A7" s="16"/>
-      <c r="B7" s="1">
+    <row r="7" s="2" customFormat="1" ht="31" spans="1:34">
+      <c r="A7" s="20"/>
+      <c r="B7" s="2">
         <v>5</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="7" t="s">
+      <c r="C7" s="14"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="27"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="34"/>
       <c r="L7"/>
       <c r="M7"/>
       <c r="N7"/>
@@ -1858,29 +2053,30 @@
       <c r="AG7"/>
       <c r="AH7"/>
     </row>
-    <row r="8" s="1" customFormat="1" ht="31.2" spans="1:34">
-      <c r="A8" s="16"/>
-      <c r="B8" s="1">
+    <row r="8" s="2" customFormat="1" ht="31" spans="1:34">
+      <c r="A8" s="20"/>
+      <c r="B8" s="2">
         <v>6</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="7" t="s">
+      <c r="C8" s="14"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="27"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="34"/>
       <c r="L8"/>
       <c r="M8"/>
       <c r="N8"/>
@@ -1905,29 +2101,30 @@
       <c r="AG8"/>
       <c r="AH8"/>
     </row>
-    <row r="9" s="1" customFormat="1" ht="31.2" spans="1:34">
-      <c r="A9" s="16"/>
-      <c r="B9" s="1">
+    <row r="9" s="2" customFormat="1" ht="31" spans="1:34">
+      <c r="A9" s="20"/>
+      <c r="B9" s="2">
         <v>7</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="7" t="s">
+      <c r="C9" s="14"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="G9" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="27"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="34"/>
       <c r="L9"/>
       <c r="M9"/>
       <c r="N9"/>
@@ -1952,29 +2149,30 @@
       <c r="AG9"/>
       <c r="AH9"/>
     </row>
-    <row r="10" s="1" customFormat="1" ht="31.2" spans="1:34">
-      <c r="A10" s="16"/>
-      <c r="B10" s="1">
+    <row r="10" s="2" customFormat="1" ht="31" spans="1:34">
+      <c r="A10" s="20"/>
+      <c r="B10" s="2">
         <v>8</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="7" t="s">
+      <c r="C10" s="14"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="G10" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I10" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="K10" s="27"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="34"/>
       <c r="L10"/>
       <c r="M10"/>
       <c r="N10"/>
@@ -1999,26 +2197,28 @@
       <c r="AG10"/>
       <c r="AH10"/>
     </row>
-    <row r="11" s="1" customFormat="1" ht="28.8" spans="1:34">
-      <c r="A11" s="16"/>
-      <c r="B11" s="1">
+    <row r="11" s="2" customFormat="1" ht="29" spans="1:34">
+      <c r="A11" s="20"/>
+      <c r="B11" s="2">
         <v>9</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="7" t="s">
+      <c r="C11" s="14"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="G11" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="K11" s="27"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="34"/>
       <c r="L11"/>
       <c r="M11"/>
       <c r="N11"/>
@@ -2043,17 +2243,20 @@
       <c r="AG11"/>
       <c r="AH11"/>
     </row>
-    <row r="12" s="1" customFormat="1" ht="15.6" spans="1:34">
-      <c r="A12" s="16"/>
-      <c r="B12" s="1">
+    <row r="12" s="2" customFormat="1" ht="15.5" spans="1:34">
+      <c r="A12" s="20"/>
+      <c r="B12" s="2">
         <v>10</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="21"/>
-      <c r="K12" s="27"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="34"/>
       <c r="L12"/>
       <c r="M12"/>
       <c r="N12"/>
@@ -2078,17 +2281,20 @@
       <c r="AG12"/>
       <c r="AH12"/>
     </row>
-    <row r="13" s="1" customFormat="1" ht="15.6" spans="1:34">
-      <c r="A13" s="16"/>
-      <c r="B13" s="1">
+    <row r="13" s="2" customFormat="1" ht="15.5" spans="1:34">
+      <c r="A13" s="20"/>
+      <c r="B13" s="2">
         <v>11</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="21"/>
-      <c r="K13" s="27"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="34"/>
       <c r="L13"/>
       <c r="M13"/>
       <c r="N13"/>
@@ -2113,621 +2319,726 @@
       <c r="AG13"/>
       <c r="AH13"/>
     </row>
-    <row r="14" customFormat="1" ht="15.6" spans="1:11">
-      <c r="A14" s="22"/>
-      <c r="B14" s="23">
+    <row r="14" customFormat="1" ht="15.5" spans="1:11">
+      <c r="A14" s="28"/>
+      <c r="B14" s="2">
         <v>12</v>
       </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="33"/>
-    </row>
-    <row r="15" ht="100.8" spans="1:11">
-      <c r="A15" s="25" t="s">
+      <c r="C14" s="14"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="57"/>
+    </row>
+    <row r="15" ht="116" spans="1:11">
+      <c r="A15" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="24">
+      <c r="B15" s="32">
         <v>13</v>
       </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="7" t="s">
+      <c r="C15" s="14"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F15" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="G15" s="26" t="s">
+      <c r="G15" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="H15" s="24" t="s">
+      <c r="H15" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="I15" s="24" t="s">
+      <c r="I15" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="J15" s="24"/>
-      <c r="K15" s="33"/>
-    </row>
-    <row r="16" ht="100.8" spans="1:11">
-      <c r="A16" s="25"/>
-      <c r="B16" s="1">
+      <c r="J15" s="58"/>
+      <c r="K15" s="57"/>
+    </row>
+    <row r="16" ht="101.5" spans="1:11">
+      <c r="A16" s="31"/>
+      <c r="B16" s="2">
         <v>14</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="7" t="s">
+      <c r="C16" s="14"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="G16" s="26" t="s">
+      <c r="G16" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="H16" s="27" t="s">
+      <c r="H16" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="I16" s="24" t="s">
+      <c r="I16" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="J16" s="1"/>
-      <c r="K16" s="27"/>
-    </row>
-    <row r="17" ht="100.8" spans="1:11">
-      <c r="A17" s="25"/>
-      <c r="B17" s="1">
+      <c r="J16" s="58"/>
+      <c r="K16" s="34"/>
+    </row>
+    <row r="17" ht="116" spans="1:11">
+      <c r="A17" s="31"/>
+      <c r="B17" s="2">
         <v>15</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="7" t="s">
+      <c r="C17" s="14"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="G17" s="26" t="s">
+      <c r="G17" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="27" t="s">
+      <c r="H17" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="I17" s="24" t="s">
+      <c r="I17" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="J17" s="1"/>
-      <c r="K17" s="27"/>
-    </row>
-    <row r="18" ht="100.8" spans="1:11">
-      <c r="A18" s="25"/>
-      <c r="B18" s="1">
+      <c r="J17" s="58"/>
+      <c r="K17" s="34"/>
+    </row>
+    <row r="18" ht="116" spans="1:11">
+      <c r="A18" s="31"/>
+      <c r="B18" s="2">
         <v>16</v>
       </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="7" t="s">
+      <c r="C18" s="14"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="F18" s="13" t="s">
+      <c r="F18" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="G18" s="26" t="s">
+      <c r="G18" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="H18" s="27" t="s">
+      <c r="H18" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="I18" s="24" t="s">
+      <c r="I18" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="J18" s="1"/>
-      <c r="K18" s="27"/>
-    </row>
-    <row r="19" ht="100.8" spans="1:11">
-      <c r="A19" s="25"/>
-      <c r="B19" s="1">
+      <c r="J18" s="58"/>
+      <c r="K18" s="34"/>
+    </row>
+    <row r="19" ht="116" spans="1:11">
+      <c r="A19" s="31"/>
+      <c r="B19" s="2">
         <v>17</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="7" t="s">
+      <c r="C19" s="14"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="G19" s="26" t="s">
+      <c r="G19" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="H19" s="27" t="s">
+      <c r="H19" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="I19" s="24" t="s">
+      <c r="I19" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="J19" s="1"/>
-      <c r="K19" s="27"/>
-    </row>
-    <row r="20" ht="100.8" spans="1:11">
-      <c r="A20" s="25"/>
-      <c r="B20" s="1">
+      <c r="J19" s="58"/>
+      <c r="K19" s="34"/>
+    </row>
+    <row r="20" ht="116" spans="1:11">
+      <c r="A20" s="31"/>
+      <c r="B20" s="2">
         <v>18</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="7" t="s">
+      <c r="C20" s="14"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="G20" s="26" t="s">
+      <c r="G20" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="H20" s="27" t="s">
+      <c r="H20" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="I20" s="24" t="s">
+      <c r="I20" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="J20" s="1"/>
-      <c r="K20" s="27"/>
-    </row>
-    <row r="21" ht="100.8" spans="1:11">
-      <c r="A21" s="25"/>
-      <c r="B21" s="1">
+      <c r="J20" s="58"/>
+      <c r="K20" s="34"/>
+    </row>
+    <row r="21" ht="101.5" spans="1:11">
+      <c r="A21" s="31"/>
+      <c r="B21" s="2">
         <v>19</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="7" t="s">
+      <c r="C21" s="14"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="F21" s="13" t="s">
+      <c r="F21" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="G21" s="26" t="s">
+      <c r="G21" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="H21" s="27" t="s">
+      <c r="H21" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="I21" s="24" t="s">
+      <c r="I21" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="J21" s="1"/>
-      <c r="K21" s="27"/>
-    </row>
-    <row r="22" ht="100.8" spans="1:11">
-      <c r="A22" s="25"/>
-      <c r="B22" s="1">
+      <c r="J21" s="58"/>
+      <c r="K21" s="34"/>
+    </row>
+    <row r="22" ht="101.5" spans="1:11">
+      <c r="A22" s="31"/>
+      <c r="B22" s="2">
         <v>20</v>
       </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="7" t="s">
+      <c r="C22" s="14"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="F22" s="13" t="s">
+      <c r="F22" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="G22" s="26" t="s">
+      <c r="G22" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="H22" s="27" t="s">
+      <c r="H22" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="I22" s="24" t="s">
+      <c r="I22" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="J22" s="1"/>
-      <c r="K22" s="27"/>
-    </row>
-    <row r="23" ht="28.8" spans="1:11">
-      <c r="A23" s="25"/>
-      <c r="B23" s="1">
+      <c r="J22" s="58"/>
+      <c r="K22" s="34"/>
+    </row>
+    <row r="23" ht="29" spans="1:11">
+      <c r="A23" s="31"/>
+      <c r="B23" s="2">
         <v>21</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="7" t="s">
+      <c r="C23" s="14"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="F23" s="13" t="s">
+      <c r="F23" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="G23" s="26" t="s">
+      <c r="G23" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="H23" s="27" t="s">
+      <c r="H23" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="I23" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="J23" s="1"/>
-      <c r="K23" s="27"/>
-    </row>
-    <row r="24" ht="28.8" spans="1:11">
-      <c r="A24" s="25"/>
-      <c r="B24" s="1">
+      <c r="J23" s="58"/>
+      <c r="K23" s="34"/>
+    </row>
+    <row r="24" ht="29" spans="1:11">
+      <c r="A24" s="31"/>
+      <c r="B24" s="2">
         <v>22</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="7" t="s">
+      <c r="C24" s="14"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="F24" s="13" t="s">
+      <c r="F24" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="G24" s="26" t="s">
+      <c r="G24" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="H24" s="27" t="s">
+      <c r="H24" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="I24" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="J24" s="1"/>
-      <c r="K24" s="27"/>
-    </row>
-    <row r="25" ht="43.2" spans="1:11">
-      <c r="A25" s="25"/>
-      <c r="B25" s="1">
+      <c r="J24" s="58"/>
+      <c r="K24" s="34"/>
+    </row>
+    <row r="25" ht="43.5" spans="1:11">
+      <c r="A25" s="31"/>
+      <c r="B25" s="2">
         <v>23</v>
       </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="7" t="s">
+      <c r="C25" s="14"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="F25" s="13" t="s">
+      <c r="F25" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="G25" s="26" t="s">
+      <c r="G25" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="H25" s="27" t="s">
+      <c r="H25" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="I25" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="J25" s="1"/>
-      <c r="K25" s="27"/>
-    </row>
-    <row r="26" ht="15.6" spans="1:11">
-      <c r="A26" s="25"/>
-      <c r="B26" s="1">
+      <c r="J25" s="58"/>
+      <c r="K25" s="34"/>
+    </row>
+    <row r="26" ht="15.5" spans="1:11">
+      <c r="A26" s="31"/>
+      <c r="B26" s="2">
         <v>24</v>
       </c>
-      <c r="C26" s="11"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="7" t="s">
+      <c r="C26" s="14"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="F26" s="13" t="s">
+      <c r="F26" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="G26" s="26" t="s">
+      <c r="G26" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="H26" s="27" t="s">
+      <c r="H26" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="I26" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="J26" s="1"/>
-      <c r="K26" s="27"/>
-    </row>
-    <row r="27" ht="15.6" spans="1:11">
-      <c r="A27" s="25"/>
-      <c r="B27" s="1">
+      <c r="J26" s="58"/>
+      <c r="K26" s="34"/>
+    </row>
+    <row r="27" ht="15.5" spans="1:11">
+      <c r="A27" s="31"/>
+      <c r="B27" s="2">
         <v>25</v>
       </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="7" t="s">
+      <c r="C27" s="14"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="F27" s="13" t="s">
+      <c r="F27" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="G27" s="26" t="s">
+      <c r="G27" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="H27" s="27" t="s">
+      <c r="H27" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="I27" s="1" t="s">
+      <c r="I27" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="J27" s="1"/>
-      <c r="K27" s="27"/>
-    </row>
-    <row r="28" ht="15.6" spans="1:11">
-      <c r="A28" s="25"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="27"/>
+      <c r="J27" s="58"/>
+      <c r="K27" s="34"/>
+    </row>
+    <row r="28" ht="15.5" spans="1:11">
+      <c r="A28" s="31"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="58"/>
+      <c r="J28" s="58"/>
+      <c r="K28" s="34"/>
     </row>
     <row r="29" ht="114" customHeight="1" spans="1:11">
-      <c r="A29" s="28"/>
-      <c r="B29" s="1" t="s">
+      <c r="A29" s="35"/>
+      <c r="B29" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C29" s="11"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="27"/>
-    </row>
-    <row r="30" ht="43.2" spans="1:11">
-      <c r="A30" s="29" t="s">
+      <c r="C29" s="14"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="58"/>
+      <c r="J29" s="58"/>
+      <c r="K29" s="34"/>
+    </row>
+    <row r="30" ht="105" customHeight="1" spans="1:11">
+      <c r="A30" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="B30" s="1">
-        <v>15</v>
-      </c>
-      <c r="C30" s="11"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="13" t="s">
+      <c r="B30" s="2">
+        <v>26</v>
+      </c>
+      <c r="C30" s="14"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="G30" s="21"/>
-      <c r="H30" s="27" t="s">
+      <c r="F30" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="27"/>
-    </row>
-    <row r="31" ht="28.8" spans="1:11">
-      <c r="A31" s="25"/>
-      <c r="B31" s="1">
-        <v>16</v>
-      </c>
-      <c r="C31" s="11"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="13" t="s">
+      <c r="G30" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="G31" s="21"/>
-      <c r="H31" s="27" t="s">
+      <c r="H30" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="27"/>
-    </row>
-    <row r="32" ht="43.2" spans="1:11">
-      <c r="A32" s="28"/>
-      <c r="B32" s="1">
-        <v>17</v>
-      </c>
-      <c r="C32" s="11"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="13" t="s">
+      <c r="I30" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="J30" s="60"/>
+      <c r="K30" s="40"/>
+    </row>
+    <row r="31" ht="65" customHeight="1" spans="1:11">
+      <c r="A31" s="41"/>
+      <c r="B31" s="2">
+        <v>27</v>
+      </c>
+      <c r="C31" s="14"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="G32" s="21"/>
-      <c r="H32" s="1" t="s">
+      <c r="F31" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="27"/>
-    </row>
-    <row r="33" ht="15.6" spans="1:11">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="7"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="27"/>
-    </row>
-    <row r="34" ht="15.6" spans="1:11">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="7"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="27"/>
-    </row>
-    <row r="35" ht="15.6" spans="1:11">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="7"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="27"/>
-    </row>
-    <row r="36" ht="15.6" spans="1:11">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="7"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="27"/>
-    </row>
-    <row r="37" ht="15.6" spans="1:11">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="7"/>
-      <c r="G37" s="21"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="27"/>
-    </row>
-    <row r="38" ht="15.6" spans="1:11">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="7"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="27"/>
-    </row>
-    <row r="39" ht="15.6" spans="1:11">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="7"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="27"/>
-    </row>
-    <row r="40" ht="15.6" spans="1:11">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="11"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="7"/>
-      <c r="G40" s="21"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="27"/>
-    </row>
-    <row r="41" ht="15.6" spans="1:11">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="7"/>
-      <c r="G41" s="21"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="27"/>
-    </row>
-    <row r="42" ht="15.6" spans="1:11">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="7"/>
-      <c r="G42" s="21"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="27"/>
-    </row>
-    <row r="43" ht="15.6" spans="1:11">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="7"/>
-      <c r="G43" s="21"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="27"/>
-    </row>
-    <row r="44" ht="15.6" spans="1:11">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="7"/>
-      <c r="G44" s="21"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="27"/>
-    </row>
-    <row r="45" ht="15.6" spans="1:11">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="7"/>
-      <c r="G45" s="21"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-      <c r="K45" s="27"/>
-    </row>
-    <row r="46" ht="15.6" spans="1:11">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="7"/>
-      <c r="G46" s="21"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="27"/>
-    </row>
-    <row r="47" ht="15.6" spans="1:11">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="7"/>
-      <c r="G47" s="21"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="27"/>
+      <c r="G31" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="H31" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="I31" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="J31" s="56"/>
+      <c r="K31" s="34"/>
+    </row>
+    <row r="32" ht="44" customHeight="1" spans="1:11">
+      <c r="A32" s="41"/>
+      <c r="B32" s="2">
+        <v>28</v>
+      </c>
+      <c r="C32" s="14"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="F32" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="G32" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="H32" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="I32" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="J32" s="60"/>
+      <c r="K32" s="40"/>
+    </row>
+    <row r="33" ht="47" customHeight="1" spans="1:11">
+      <c r="A33" s="41"/>
+      <c r="B33" s="2">
+        <v>29</v>
+      </c>
+      <c r="C33" s="14"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G33" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="H33" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="I33" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="J33" s="56"/>
+      <c r="K33" s="34"/>
+    </row>
+    <row r="34" ht="28" customHeight="1" spans="1:11">
+      <c r="A34" s="41"/>
+      <c r="B34" s="2">
+        <v>30</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="F34" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="G34" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="H34" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="I34" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="J34" s="60"/>
+      <c r="K34" s="40"/>
+    </row>
+    <row r="35" ht="42" customHeight="1" spans="1:11">
+      <c r="A35" s="41"/>
+      <c r="B35" s="2">
+        <v>31</v>
+      </c>
+      <c r="C35" s="14"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G35" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="H35" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="I35" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="J35" s="56"/>
+      <c r="K35" s="34"/>
+    </row>
+    <row r="36" ht="35" customHeight="1" spans="1:11">
+      <c r="A36" s="47"/>
+      <c r="B36" s="2">
+        <v>32</v>
+      </c>
+      <c r="C36" s="14"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="F36" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="G36" s="46" t="s">
+        <v>123</v>
+      </c>
+      <c r="H36" s="48" t="s">
+        <v>124</v>
+      </c>
+      <c r="I36" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="J36" s="60"/>
+      <c r="K36" s="40"/>
+    </row>
+    <row r="37" ht="15.5" spans="1:11">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="24"/>
+      <c r="K37" s="34"/>
+    </row>
+    <row r="38" ht="15.5" spans="1:11">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="24"/>
+      <c r="J38" s="24"/>
+      <c r="K38" s="34"/>
+    </row>
+    <row r="39" ht="15.5" spans="1:11">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="24"/>
+      <c r="J39" s="24"/>
+      <c r="K39" s="34"/>
+    </row>
+    <row r="40" ht="15.5" spans="1:11">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="24"/>
+      <c r="I40" s="24"/>
+      <c r="J40" s="24"/>
+      <c r="K40" s="34"/>
+    </row>
+    <row r="41" ht="15.5" spans="1:11">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="24"/>
+      <c r="J41" s="24"/>
+      <c r="K41" s="34"/>
+    </row>
+    <row r="42" ht="15.5" spans="1:11">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="16"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="24"/>
+      <c r="J42" s="24"/>
+      <c r="K42" s="34"/>
+    </row>
+    <row r="43" ht="15.5" spans="1:11">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="16"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="24"/>
+      <c r="I43" s="24"/>
+      <c r="J43" s="24"/>
+      <c r="K43" s="34"/>
+    </row>
+    <row r="44" ht="15.5" spans="1:11">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="16"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="24"/>
+      <c r="I44" s="24"/>
+      <c r="J44" s="24"/>
+      <c r="K44" s="34"/>
+    </row>
+    <row r="45" ht="15.5" spans="1:11">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="16"/>
+      <c r="G45" s="27"/>
+      <c r="H45" s="24"/>
+      <c r="I45" s="24"/>
+      <c r="J45" s="24"/>
+      <c r="K45" s="34"/>
+    </row>
+    <row r="46" ht="15.5" spans="1:11">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="16"/>
+      <c r="G46" s="27"/>
+      <c r="H46" s="24"/>
+      <c r="I46" s="24"/>
+      <c r="J46" s="24"/>
+      <c r="K46" s="34"/>
+    </row>
+    <row r="47" ht="15.5" spans="1:11">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="49"/>
+      <c r="D47" s="50"/>
+      <c r="E47" s="16"/>
+      <c r="G47" s="27"/>
+      <c r="H47" s="24"/>
+      <c r="I47" s="24"/>
+      <c r="J47" s="24"/>
+      <c r="K47" s="34"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="35">
     <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="I36:J36"/>
     <mergeCell ref="A3:A13"/>
     <mergeCell ref="A15:A29"/>
-    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A30:A36"/>
     <mergeCell ref="C2:D47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>